<commit_message>
Add new files for exp_id6
</commit_message>
<xml_diff>
--- a/experiments/exp_id6_ApplicationAnalysis/exper_id6_selectedStats_2hops.xlsx
+++ b/experiments/exp_id6_ApplicationAnalysis/exper_id6_selectedStats_2hops.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Qwanta\qwanta\experiments\exp_id2_strategies_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Qwanta\qwanta\experiments\exp_id6_ApplicationAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C820B46-8C2C-4A4B-91C4-4BE7D2D52699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA59303-AC3B-403F-95F3-E313B7F40AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{CC982C2F-A1FA-4C57-B573-5585ACEA208F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{CC982C2F-A1FA-4C57-B573-5585ACEA208F}"/>
   </bookViews>
   <sheets>
     <sheet name="0G" sheetId="1" r:id="rId1"/>
-    <sheet name="1G-Ss-Dp" sheetId="2" r:id="rId2"/>
-    <sheet name="2G-NonLocalCNOT" sheetId="3" r:id="rId3"/>
-    <sheet name="1-2G-DirectedEncoded" sheetId="4" r:id="rId4"/>
-    <sheet name="HG-END2ENDPurifiedEncoded" sheetId="7" r:id="rId5"/>
-    <sheet name="1-2G-DirectedEncoded-Perfect" sheetId="6" r:id="rId6"/>
-    <sheet name="2G-NonLocalCNOT-Perfect" sheetId="5" r:id="rId7"/>
+    <sheet name="E2E-1G-Ss-Dp" sheetId="8" r:id="rId2"/>
+    <sheet name="1G-Ss-Dp" sheetId="2" r:id="rId3"/>
+    <sheet name="2G-NonLocalCNOT" sheetId="3" r:id="rId4"/>
+    <sheet name="1-2G-DirectedEncoded" sheetId="4" r:id="rId5"/>
+    <sheet name="HG-END2ENDPurifiedEncoded" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="27">
   <si>
     <t>Main Process</t>
   </si>
@@ -116,9 +115,6 @@
   </si>
   <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>Perfect</t>
   </si>
   <si>
     <t>Swapped</t>
@@ -477,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AC36BB-5461-4A26-A1F4-F72881C6052F}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -593,11 +589,151 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ADC67AC-2FF6-4BFD-ACB7-682FFC866A4B}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="26.625" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>9000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED893E88-3F8D-451C-B567-0170D15222A3}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A5" sqref="A5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -751,7 +887,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3EB34F-8007-43F3-80B4-B769DD5BE88E}">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -915,7 +1051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDAFEEC-62BD-413F-97CB-9620B957E55F}">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -1121,11 +1257,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26A1926-2A77-402C-B808-3358938D726F}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1211,7 +1347,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -1228,7 +1364,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -1278,388 +1414,6 @@
       </c>
       <c r="F7" t="s">
         <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CFDB072-F5B0-45B1-BE7D-13669E6F5DB2}">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>9000</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6214153D-35EB-45D8-BA19-74487CCBE690}">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.375" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="7" max="7" width="16.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
-        <v>9000</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add name for experiment and fix label record
</commit_message>
<xml_diff>
--- a/experiments/exp_id6_ApplicationAnalysis/exper_id6_selectedStats_2hops.xlsx
+++ b/experiments/exp_id6_ApplicationAnalysis/exper_id6_selectedStats_2hops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Qwanta\qwanta\experiments\exp_id6_ApplicationAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA59303-AC3B-403F-95F3-E313B7F40AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39443976-4F83-4B7B-A198-068C268DDD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{CC982C2F-A1FA-4C57-B573-5585ACEA208F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="28">
   <si>
     <t>Main Process</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Swapped</t>
+  </si>
+  <si>
+    <t>swapped</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -593,7 +596,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -677,7 +680,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -694,10 +697,10 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
       </c>
       <c r="G5" t="s">
         <v>15</v>
@@ -714,7 +717,7 @@
         <v>9000</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -1056,7 +1059,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:F9"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1262,7 +1265,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix data extraction process
</commit_message>
<xml_diff>
--- a/experiments/exp_id6_ApplicationAnalysis/exper_id6_selectedStats_2hops.xlsx
+++ b/experiments/exp_id6_ApplicationAnalysis/exper_id6_selectedStats_2hops.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Qwanta\qwanta\experiments\exp_id6_ApplicationAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39443976-4F83-4B7B-A198-068C268DDD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8D07D3-FBE6-4369-A2F5-1C6D48060AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{CC982C2F-A1FA-4C57-B573-5585ACEA208F}"/>
+    <workbookView xWindow="2670" yWindow="2430" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{CC982C2F-A1FA-4C57-B573-5585ACEA208F}"/>
   </bookViews>
   <sheets>
     <sheet name="0G" sheetId="1" r:id="rId1"/>
@@ -1265,7 +1265,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>